<commit_message>
Resized fonts on gant chart
</commit_message>
<xml_diff>
--- a/Venture Proposal/EVappTL.xlsx
+++ b/Venture Proposal/EVappTL.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vlora95/Documents/GitHub/EVApp/Venture Proposal/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="0" windowWidth="19320" windowHeight="15720" tabRatio="500"/>
+    <workbookView xWindow="28780" yWindow="-3480" windowWidth="29780" windowHeight="18180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,6 +114,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -133,10 +143,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="3200"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="3200"/>
               <a:t>EVApp Timeline</a:t>
             </a:r>
           </a:p>
@@ -422,12 +432,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2102946760"/>
-        <c:axId val="2102949736"/>
+        <c:axId val="-2128891072"/>
+        <c:axId val="-2128886576"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2102946760"/>
+        <c:axId val="-2128891072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,10 +450,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Tasks</a:t>
                 </a:r>
               </a:p>
@@ -456,7 +466,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102949736"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2128886576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -464,7 +484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102949736"/>
+        <c:axId val="-2128886576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42535.0"/>
@@ -480,10 +500,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Dates</a:t>
                 </a:r>
               </a:p>
@@ -496,7 +516,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102946760"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2128891072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -505,6 +535,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -528,10 +568,10 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -881,9 +921,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -897,7 +937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -908,7 +948,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -919,7 +959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -930,7 +970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -941,7 +981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -952,7 +992,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -963,7 +1003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -974,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -985,7 +1025,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1000,10 +1040,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>